<commit_message>
progress with nat acc expenditure categories
</commit_message>
<xml_diff>
--- a/Database setup/Expenditure imputation/Crosswalk POF - National Accounts.xlsx
+++ b/Database setup/Expenditure imputation/Crosswalk POF - National Accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.perez\Desktop\Projetos\POF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.perez\Downloads\brasmod\brasmod\Database setup\Expenditure imputation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -645,7 +645,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5981" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5991" sqref="C5991:C6000"/>
+      <selection pane="bottomLeft" activeCell="G6001" sqref="G6001"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>